<commit_message>
v2.0.1 Add templates and automate mailing process
</commit_message>
<xml_diff>
--- a/correos/correos_FINAL.xlsx
+++ b/correos/correos_FINAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29816"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educacionpublica-my.sharepoint.com/personal/alonso_arrano_dep_cl/Documents/2024/SAE - Anotate en la lista/reporteria_ael/correos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="11_AD4D2F04E46CFB4ACB3E20CA8550FF6C693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77B69095-D774-4832-9219-06D538D73CB0}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="11_AD4D2F04E46CFB4ACB3E20CA8550FF6C693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E6ED773-D2D1-4669-8DAB-3429CC09303A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="10965" yWindow="6570" windowWidth="14400" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$A$37</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,42 +40,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="222">
+  <si>
+    <t>Tipo_SLEP</t>
+  </si>
   <si>
     <t>SLEP</t>
   </si>
   <si>
+    <t>Nombre Completo</t>
+  </si>
+  <si>
     <t>Nombre</t>
   </si>
   <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>RUT</t>
+  </si>
+  <si>
     <t>correo</t>
   </si>
   <si>
+    <t>copia</t>
+  </si>
+  <si>
     <t>archivo</t>
   </si>
   <si>
+    <t>Antiguo</t>
+  </si>
+  <si>
     <t>Llanquihue</t>
   </si>
   <si>
     <t>Ana Galleguillos</t>
   </si>
   <si>
+    <t>Galleguillos</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>ana.galleguillos@slepllanquihue.cl</t>
   </si>
   <si>
+    <t>jocelyn.almonacid@slepllanquihue.cl</t>
+  </si>
+  <si>
+    <t>reporte_llanquihue.html</t>
+  </si>
+  <si>
     <t>Chiloé</t>
   </si>
   <si>
     <t>Eduardo Sarmiento</t>
   </si>
   <si>
+    <t>Sarmiento</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>15.904.815-2</t>
+  </si>
+  <si>
     <t>Altircio.sarmiento@slepchiloe.gob.cl</t>
   </si>
   <si>
-    <t>copia</t>
-  </si>
-  <si>
-    <t>luis.gajardo@slepchiloe.gob.cl; camilo.elgueta@slepchiloe.gob.cl</t>
+    <t>reporte_Chiloé.html</t>
   </si>
   <si>
     <t>Valdivia</t>
@@ -84,19 +123,31 @@
     <t>Jasmín San Martin</t>
   </si>
   <si>
+    <t>San Martin</t>
+  </si>
+  <si>
     <t>jasmin.sanmartin@slepvaldivia.gob.cl</t>
   </si>
   <si>
+    <t>reporte_valdivia.html</t>
+  </si>
+  <si>
     <t>Santa Rosa</t>
   </si>
   <si>
+    <t>Jenson Aleman</t>
+  </si>
+  <si>
+    <t>Aleman</t>
+  </si>
+  <si>
+    <t>jenson.aleman@slepsantarosa.gob.cl</t>
+  </si>
+  <si>
     <t>josefina.abarzua@slepsantarosa.gob.cl</t>
   </si>
   <si>
-    <t>Jenson Aleman</t>
-  </si>
-  <si>
-    <t>jenson.aleman@slepsantarosa.gob.cl</t>
+    <t>reporte_santa_rosa.html</t>
   </si>
   <si>
     <t>Santa Corina</t>
@@ -105,52 +156,91 @@
     <t>Juan Durán</t>
   </si>
   <si>
+    <t>Durán</t>
+  </si>
+  <si>
     <t>juan.duran@slepsantacorina.gob.cl</t>
   </si>
   <si>
+    <t>reporte_santa_corina.html</t>
+  </si>
+  <si>
     <t>Maule Costa</t>
   </si>
   <si>
     <t>Yolanda Urrutia</t>
   </si>
   <si>
+    <t>Urrutia</t>
+  </si>
+  <si>
     <t>yolanda.urrutia@slepmaulecosta.gob.cl</t>
   </si>
   <si>
+    <t>reporte_maule_costa.html</t>
+  </si>
+  <si>
     <t>Los Libertadores</t>
   </si>
   <si>
     <t>Manuel Coloma</t>
   </si>
   <si>
+    <t>Coloma</t>
+  </si>
+  <si>
     <t>manuel.coloma@sleploslibertadores.gob.cl</t>
   </si>
   <si>
+    <t>reporte_los_libertadores.html</t>
+  </si>
+  <si>
     <t>Licancabur</t>
   </si>
   <si>
     <t>David Cruz</t>
   </si>
   <si>
+    <t>Cruz</t>
+  </si>
+  <si>
     <t>david.cruz@sleplicancabur.cl</t>
   </si>
   <si>
+    <t>reporte_licancabur.html</t>
+  </si>
+  <si>
     <t>Andalién Costa</t>
   </si>
   <si>
+    <t>Marcela Valencia</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>13.635.015-3</t>
+  </si>
+  <si>
+    <t>marcela.valencia@slepandaliencosta.gob.cl</t>
+  </si>
+  <si>
+    <t>reporte_andalién_costa.html</t>
+  </si>
+  <si>
     <t>Del Pino</t>
   </si>
   <si>
     <t>Rodrigo Yañez</t>
   </si>
   <si>
+    <t>Yañez</t>
+  </si>
+  <si>
     <t>rodrigo.yanez@edudelpino.gob.cl</t>
   </si>
   <si>
-    <t>Marcela Valencia</t>
-  </si>
-  <si>
-    <t>marcela.valencia@slepandaliencosta.gob.cl</t>
+    <t>reporte_del_pino.html</t>
   </si>
   <si>
     <t>Punilla Cordillera</t>
@@ -159,31 +249,49 @@
     <t>Eugenio Fierro</t>
   </si>
   <si>
+    <t>Fierro</t>
+  </si>
+  <si>
     <t>eugenio.fierro@sleppunillacordillera.cl</t>
   </si>
   <si>
     <t>karla.sepulveda@sleppunillacordillera.cl</t>
   </si>
   <si>
+    <t>reporte_punilla_cordillera.html</t>
+  </si>
+  <si>
     <t>Magallanes</t>
   </si>
   <si>
     <t>Carolina Figueroa</t>
   </si>
   <si>
+    <t>Figueroa</t>
+  </si>
+  <si>
     <t>carolina.figueroa@slepmagallanes.cl</t>
   </si>
   <si>
+    <t>reporte_magallanes.html</t>
+  </si>
+  <si>
     <t>Aysen</t>
   </si>
   <si>
+    <t>Ivy Guedeney</t>
+  </si>
+  <si>
+    <t>Guedeney</t>
+  </si>
+  <si>
+    <t>ivy.guedeney@slepaysen.cl</t>
+  </si>
+  <si>
     <t>freddy.moraga@slepaysen.cl</t>
   </si>
   <si>
-    <t>Ivy Guedeney</t>
-  </si>
-  <si>
-    <t>ivy.guedeney@slepaysen.cl</t>
+    <t>reporte_aysén.html</t>
   </si>
   <si>
     <t xml:space="preserve">Iquique </t>
@@ -192,183 +300,177 @@
     <t>Mario Reyes</t>
   </si>
   <si>
+    <t>Reyes</t>
+  </si>
+  <si>
     <t>mario.reyes@slepiquique.cl</t>
   </si>
   <si>
+    <t>reporte_iquique.html</t>
+  </si>
+  <si>
     <t>Costa Araucanía</t>
   </si>
   <si>
     <t>Sandra Padilla</t>
   </si>
   <si>
+    <t>Padilla</t>
+  </si>
+  <si>
     <t>sandra.padilla@slepca.cl</t>
   </si>
   <si>
+    <t>reporte_costa_araucanía.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atacama </t>
   </si>
   <si>
     <t>Marcelo Quiroga</t>
   </si>
   <si>
+    <t>Quiroga</t>
+  </si>
+  <si>
     <t>marcelo.quiroga@slepatacama.cl</t>
   </si>
   <si>
+    <t>reporte_atacama.html</t>
+  </si>
+  <si>
     <t>Huasco</t>
   </si>
   <si>
     <t>Maryorie Alquinta</t>
   </si>
   <si>
+    <t>Alquinta</t>
+  </si>
+  <si>
     <t>maryorie.alquinta@slephuasco.cl</t>
   </si>
   <si>
+    <t>reporte_huasco.html</t>
+  </si>
+  <si>
     <t>Puerto Cordillera</t>
   </si>
   <si>
     <t>Margarita Campillo</t>
   </si>
   <si>
+    <t>Campillo</t>
+  </si>
+  <si>
     <t>margarita.campillo@slepuertocordillera.cl</t>
   </si>
   <si>
+    <t>reporte_puerto_cordillera.html</t>
+  </si>
+  <si>
     <t>Valparaíso</t>
   </si>
   <si>
     <t>Angeline castillo</t>
   </si>
   <si>
+    <t>Castillo</t>
+  </si>
+  <si>
     <t>angeline.castillo@slepvalparaiso.cl</t>
   </si>
   <si>
+    <t>reporte_valparaíso.html</t>
+  </si>
+  <si>
     <t>Barrancas</t>
   </si>
   <si>
     <t>Daniela Chamorro</t>
   </si>
   <si>
+    <t>Chamorro</t>
+  </si>
+  <si>
     <t>daniela.chamorro@slepb.cl</t>
   </si>
   <si>
+    <t>reporte_barrancas.html</t>
+  </si>
+  <si>
     <t>Gabriela Mistral</t>
   </si>
   <si>
     <t>Marta Hinojosa</t>
   </si>
   <si>
+    <t>Hinojosa</t>
+  </si>
+  <si>
     <t>marta.hinojosa@slepgm.cl</t>
   </si>
   <si>
+    <t>reporte_gabriela_mistral.html</t>
+  </si>
+  <si>
     <t>Colchagua</t>
   </si>
   <si>
     <t>Oscar Ubilla</t>
   </si>
   <si>
+    <t>Ubilla</t>
+  </si>
+  <si>
     <t>oscar.ubilla@slepcolchagua.cl</t>
   </si>
   <si>
+    <t>reporte_colchagua.html</t>
+  </si>
+  <si>
     <t>Andalién Sur</t>
   </si>
   <si>
     <t>Elena Saez</t>
   </si>
   <si>
+    <t>Saez</t>
+  </si>
+  <si>
     <t>elena.saez@andaliensur.cl</t>
   </si>
   <si>
+    <t>reporte_andalién_sur.html</t>
+  </si>
+  <si>
     <t>Chinchorro</t>
   </si>
   <si>
     <t>Carolina Aguilera</t>
   </si>
   <si>
+    <t>Aguilera</t>
+  </si>
+  <si>
     <t>carolina.aguilera@epchinchorro.cl</t>
   </si>
   <si>
     <t>shirley.villegas@epchinchorro.cl</t>
   </si>
   <si>
-    <t>Nombre Completo</t>
-  </si>
-  <si>
-    <t>reporte_llanquihue.html</t>
-  </si>
-  <si>
-    <t>reporte_valdivia.html</t>
-  </si>
-  <si>
-    <t>reporte_licancabur.html</t>
-  </si>
-  <si>
-    <t>reporte_magallanes.html</t>
-  </si>
-  <si>
-    <t>reporte_Chiloé.html</t>
-  </si>
-  <si>
-    <t>reporte_iquique.html</t>
-  </si>
-  <si>
-    <t>reporte_atacama.html</t>
-  </si>
-  <si>
-    <t>reporte_huasco.html</t>
-  </si>
-  <si>
-    <t>reporte_valparaíso.html</t>
-  </si>
-  <si>
-    <t>reporte_barrancas.html</t>
-  </si>
-  <si>
-    <t>reporte_colchagua.html</t>
-  </si>
-  <si>
     <t>reporte_chinchorro.html</t>
   </si>
   <si>
-    <t>reporte_andalién_costa.html</t>
-  </si>
-  <si>
-    <t>reporte_santa_rosa.html</t>
-  </si>
-  <si>
-    <t>reporte_santa_corina.html</t>
-  </si>
-  <si>
-    <t>reporte_maule_costa.html</t>
-  </si>
-  <si>
-    <t>reporte_los_libertadores.html</t>
-  </si>
-  <si>
-    <t>reporte_del_pino.html</t>
-  </si>
-  <si>
-    <t>reporte_punilla_cordillera.html</t>
-  </si>
-  <si>
-    <t>reporte_costa_araucanía.html</t>
-  </si>
-  <si>
-    <t>reporte_puerto_cordillera.html</t>
-  </si>
-  <si>
-    <t>reporte_gabriela_mistral.html</t>
-  </si>
-  <si>
-    <t>reporte_andalién_sur.html</t>
-  </si>
-  <si>
-    <t>reporte_aysén.html</t>
-  </si>
-  <si>
     <t>Costa Central</t>
   </si>
   <si>
     <t>Tomás Gonzalez</t>
   </si>
   <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
     <t>tomas.gonzalez@slepcostacentral.gob.cl</t>
   </si>
   <si>
@@ -378,24 +480,21 @@
     <t>Elqui</t>
   </si>
   <si>
+    <t>Rosita Zepeda</t>
+  </si>
+  <si>
+    <t>Zepeda</t>
+  </si>
+  <si>
     <t>rosita.zepeda@slepelqui.gob.cl</t>
   </si>
   <si>
-    <t>Rosita Zepeda</t>
+    <t>marco.vega@slepelqui.gob.cl</t>
   </si>
   <si>
     <t>reporte_elqui.html</t>
   </si>
   <si>
-    <t>marco.vega@slepelqui.gob.cl</t>
-  </si>
-  <si>
-    <t>Tipo_SLEP</t>
-  </si>
-  <si>
-    <t>Antiguo</t>
-  </si>
-  <si>
     <t>Nuevo</t>
   </si>
   <si>
@@ -405,13 +504,19 @@
     <t>Carolina Villagra Marín </t>
   </si>
   <si>
+    <t>Villagra</t>
+  </si>
+  <si>
+    <t>18.064.502-0</t>
+  </si>
+  <si>
     <t>carolina.villagra@sleppetorca.gob.cl </t>
   </si>
   <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>18.064.502-0</t>
+    <t>mauricio.urrutia@sleppetorca.gob.cl</t>
+  </si>
+  <si>
+    <t>reporte_petorca.html</t>
   </si>
   <si>
     <t>Los Andes</t>
@@ -420,34 +525,61 @@
     <t>Miguel Ángel Briceño</t>
   </si>
   <si>
+    <t>Briceño</t>
+  </si>
+  <si>
     <t>16.387.617-5</t>
   </si>
   <si>
     <t>miguel.briceno@sleplosandes.gob.cl</t>
   </si>
   <si>
+    <t>felipe.martinez@sleplosandes.gob.cl</t>
+  </si>
+  <si>
+    <t>reporte_los_andes.html</t>
+  </si>
+  <si>
     <t>Aconcagua</t>
   </si>
   <si>
+    <t>Claudia Cubillos</t>
+  </si>
+  <si>
+    <t>Cubillos</t>
+  </si>
+  <si>
+    <t>12.600.439-7</t>
+  </si>
+  <si>
     <t>claudia.cubillos@slepaconcagua.gob.cl</t>
   </si>
   <si>
-    <t>Claudia Cubillos</t>
-  </si>
-  <si>
-    <t>12.600.439-7</t>
+    <t>yasna.flos@slepaconcagua.gob.cl</t>
+  </si>
+  <si>
+    <t>reporte_aconcagua.html</t>
   </si>
   <si>
     <t>Puelche</t>
   </si>
   <si>
-    <t>Javiera Marisol Rivas González</t>
-  </si>
-  <si>
-    <t>20.022.319-5</t>
-  </si>
-  <si>
-    <t>javiera.rivas@sleppuelche.gob.cl</t>
+    <t>Iván Alejandro Ramírez Hidalgo</t>
+  </si>
+  <si>
+    <t>Ramírez</t>
+  </si>
+  <si>
+    <t>9.488.256-7</t>
+  </si>
+  <si>
+    <t>Ivan.ramirez@sleppuelche.gob.cl</t>
+  </si>
+  <si>
+    <t>rossemarie.sanchez@sleppuelche.gob.cl</t>
+  </si>
+  <si>
+    <t>reporte_puelche.html</t>
   </si>
   <si>
     <t>Los Álamos</t>
@@ -456,45 +588,39 @@
     <t>Claudio Wilson Valenzuela</t>
   </si>
   <si>
+    <t>Valenzuela</t>
+  </si>
+  <si>
+    <t>12.790.916-4 </t>
+  </si>
+  <si>
     <t>claudio.wilson@sleplosalamos.gob.cl</t>
   </si>
   <si>
-    <t>reporte_los_andes.html</t>
-  </si>
-  <si>
-    <t>reporte_aconcagua.html</t>
-  </si>
-  <si>
-    <t>reporte_puelche.html</t>
+    <t>ximena.valenzuela@sleplosalamos.gob.cl</t>
   </si>
   <si>
     <t>reporte_los_álamos.html</t>
   </si>
   <si>
-    <t>Genero</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>reporte_petorca.html</t>
-  </si>
-  <si>
     <t>Marga Marga</t>
   </si>
   <si>
     <t>Avelino Castro</t>
   </si>
   <si>
+    <t>Castro</t>
+  </si>
+  <si>
     <t>13.988.411-6</t>
   </si>
   <si>
     <t>avelino.castro@slepmargamarga.gob.cl</t>
   </si>
   <si>
+    <t>jorge.manchini@slepmargamarga.gob.cl</t>
+  </si>
+  <si>
     <t>reporte_marga_marga.html</t>
   </si>
   <si>
@@ -504,12 +630,18 @@
     <t>Emilia Bustos</t>
   </si>
   <si>
+    <t>Bustos</t>
+  </si>
+  <si>
     <t>18.933.093-6</t>
   </si>
   <si>
     <t>Emilia.Bustos@sleplosparques.gob.cl</t>
   </si>
   <si>
+    <t>flavia.fiabane@sleplosparques.gob.cl</t>
+  </si>
+  <si>
     <t>reporte_los_parques.html</t>
   </si>
   <si>
@@ -519,147 +651,42 @@
     <t>Araceli Nuñez Chavera</t>
   </si>
   <si>
+    <t>Nuñez</t>
+  </si>
+  <si>
     <t>15.006.991-2</t>
   </si>
   <si>
     <t>araceli.nunez@sleptamarugal.gob.cl</t>
   </si>
   <si>
+    <t>samuel.diaz@sleptamarugal.gob.cl</t>
+  </si>
+  <si>
     <t>reporte_tamarugal.html</t>
   </si>
   <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Galleguillos</t>
-  </si>
-  <si>
-    <t>Sarmiento</t>
-  </si>
-  <si>
-    <t>Aleman</t>
-  </si>
-  <si>
-    <t>Durán</t>
-  </si>
-  <si>
-    <t>Urrutia</t>
-  </si>
-  <si>
-    <t>Coloma</t>
-  </si>
-  <si>
-    <t>Cruz</t>
-  </si>
-  <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>Yañez</t>
-  </si>
-  <si>
-    <t>Fierro</t>
-  </si>
-  <si>
-    <t>Figueroa</t>
-  </si>
-  <si>
-    <t>Guedeney</t>
-  </si>
-  <si>
-    <t>Reyes</t>
-  </si>
-  <si>
-    <t>Padilla</t>
-  </si>
-  <si>
-    <t>Quiroga</t>
-  </si>
-  <si>
-    <t>Alquinta</t>
-  </si>
-  <si>
-    <t>Campillo</t>
-  </si>
-  <si>
-    <t>Chamorro</t>
-  </si>
-  <si>
-    <t>Hinojosa</t>
-  </si>
-  <si>
-    <t>Ubilla</t>
-  </si>
-  <si>
-    <t>Saez</t>
-  </si>
-  <si>
-    <t>Aguilera</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
-    <t>Zepeda</t>
-  </si>
-  <si>
-    <t>Briceño</t>
-  </si>
-  <si>
-    <t>Cubillos</t>
-  </si>
-  <si>
-    <t>Valenzuela</t>
-  </si>
-  <si>
-    <t>Castro</t>
-  </si>
-  <si>
-    <t>San Martin</t>
-  </si>
-  <si>
-    <t>Castillo</t>
-  </si>
-  <si>
-    <t>Villagra</t>
-  </si>
-  <si>
-    <t>Rivas</t>
-  </si>
-  <si>
-    <t>Bustos</t>
-  </si>
-  <si>
-    <t>Nuñez</t>
-  </si>
-  <si>
-    <t>15.904.815-2</t>
-  </si>
-  <si>
-    <t>13.635.015-3</t>
-  </si>
-  <si>
-    <t>12.790.916-4 </t>
-  </si>
-  <si>
     <t>Santiago Centro</t>
   </si>
   <si>
+    <t>Natalia balboa</t>
+  </si>
+  <si>
+    <t>Balboa</t>
+  </si>
+  <si>
+    <t>18.383.962-4</t>
+  </si>
+  <si>
+    <t>natalia.balboa@slepsantiagocentro.gob.cl</t>
+  </si>
+  <si>
+    <t>juan.saez@slepsantiagocentro.gob.cl</t>
+  </si>
+  <si>
     <t>reporte_santiago_centro.html</t>
   </si>
   <si>
-    <t>jocelyn.almonacid@slepllanquihue.cl</t>
-  </si>
-  <si>
-    <t>natalia.balboa@slepsantiagocentro.gob.cl</t>
-  </si>
-  <si>
-    <t>Natalia balboa</t>
-  </si>
-  <si>
-    <t>Balboa</t>
-  </si>
-  <si>
     <t>Valle Diguillín</t>
   </si>
   <si>
@@ -669,26 +696,23 @@
     <t>Ramirez</t>
   </si>
   <si>
+    <t>17.748.655-8</t>
+  </si>
+  <si>
     <t>camila.ramirez@slepvallediguillin.gob.cl</t>
   </si>
   <si>
+    <t>sergio.hernandez@slepvallediguillin.gob.cl</t>
+  </si>
+  <si>
     <t>reporte_Valle_Diguillín.html</t>
-  </si>
-  <si>
-    <t>juan.saez@slepsantiagocentro.gob.cl</t>
-  </si>
-  <si>
-    <t>sergio.hernandez@slepvallediguillin.gob.cl</t>
-  </si>
-  <si>
-    <t>mauricio.urrutia@sleppetorca.gob.cl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,8 +767,14 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -757,8 +787,20 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -781,12 +823,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -836,92 +938,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1113,6 +1147,86 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1127,21 +1241,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}" name="Tabla1" displayName="Tabla1" ref="A1:J37" totalsRowShown="0" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}" name="Tabla1" displayName="Tabla1" ref="A1:J37" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A1:J37" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}"/>
   <tableColumns count="10">
-    <tableColumn id="7" xr3:uid="{81F1FDBA-6F8D-4F84-B350-BE6DAEB4513E}" name="Tipo_SLEP" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{71E197A0-A7D1-4117-A637-141CAE5153C7}" name="SLEP" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{7E154C76-62D9-49AC-8A5C-38CF45CFD1DA}" name="Nombre Completo" dataDxfId="17" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="6" xr3:uid="{B28C7421-A9F8-41E9-9CE2-9190783BC6C3}" name="Nombre" dataDxfId="16" dataCellStyle="Hipervínculo">
+    <tableColumn id="7" xr3:uid="{81F1FDBA-6F8D-4F84-B350-BE6DAEB4513E}" name="Tipo_SLEP" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{71E197A0-A7D1-4117-A637-141CAE5153C7}" name="SLEP" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{7E154C76-62D9-49AC-8A5C-38CF45CFD1DA}" name="Nombre Completo" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{B28C7421-A9F8-41E9-9CE2-9190783BC6C3}" name="Nombre" dataDxfId="6">
       <calculatedColumnFormula>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{894A323A-AFD3-40FD-BB58-2B308B6E9B79}" name="Apellido" dataDxfId="15" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="9" xr3:uid="{9E5CEF83-8F1C-47D8-9D60-176E8AC3FEA4}" name="Genero" dataDxfId="14" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="8" xr3:uid="{D31AB802-9D0A-47E2-B51A-3E1504C462E0}" name="RUT" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{BFEBADF9-4E36-4F51-BFFE-B6A3E1E4CDC8}" name="correo" dataDxfId="12" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="4" xr3:uid="{146F0A02-05F8-4FED-86F3-F5493953AC21}" name="copia" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{6F51BF54-5EDB-4B9D-B425-9871551CED2D}" name="archivo" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{894A323A-AFD3-40FD-BB58-2B308B6E9B79}" name="Apellido" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{9E5CEF83-8F1C-47D8-9D60-176E8AC3FEA4}" name="Genero" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{D31AB802-9D0A-47E2-B51A-3E1504C462E0}" name="RUT" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BFEBADF9-4E36-4F51-BFFE-B6A3E1E4CDC8}" name="correo" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{146F0A02-05F8-4FED-86F3-F5493953AC21}" name="copia" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{6F51BF54-5EDB-4B9D-B425-9871551CED2D}" name="archivo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1412,11 +1526,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -1427,1212 +1541,1235 @@
     <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="B2" s="6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Ana</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>163</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>202</v>
+        <v>16</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D3" s="6" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Eduardo</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>164</v>
+        <v>20</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>197</v>
+        <v>22</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I3" s="1"/>
       <c r="J3" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Jasmín</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Jenson</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Juan</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>166</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Yolanda</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>167</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Manuel</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>168</v>
+        <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>David</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Marcela</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>170</v>
+        <v>58</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>198</v>
+        <v>59</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Rodrigo</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Eugenio</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>172</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Carolina</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="1" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Ivy</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>174</v>
+        <v>80</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="1" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Mario</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>175</v>
+        <v>86</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Sandra</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>176</v>
+        <v>91</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="1" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Marcelo</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="1" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="D18" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Maryorie</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>178</v>
+        <v>101</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="1" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="D19" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Margarita</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>179</v>
+        <v>106</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="1" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="D20" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Angeline</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>192</v>
+        <v>111</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="1" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="D21" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Daniela</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="1" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D22" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Marta</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="1" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="D23" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Oscar</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="1" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="D24" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Elena</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="1" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="D25" s="3" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Carolina</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="1" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="5" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="D26" s="4" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Tomás</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="6" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="D27" s="4" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Rosita</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="1" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="6" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="D28" s="4" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Carolina</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" s="4" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Miguel</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Claudia</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75">
+      <c r="A31" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" s="4" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Iván</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75">
+      <c r="A32" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Claudio</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" s="4" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Avelino</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="J33" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I28" s="18" t="s">
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D34" s="4" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Emilia</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75">
+      <c r="A35" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="14" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Araceli</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75">
+      <c r="A36" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="14" t="str">
+        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
+        <v>Natalia</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I36" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" s="4" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Miguel</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" s="4" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Claudia</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" s="4" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Javiera</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" s="4" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Claudio</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D33" s="4" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Avelino</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6" t="s">
+      <c r="J36" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D34" s="4" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Emilia</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="14" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Araceli</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="D36" s="14" t="str">
-        <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
-        <v>Natalia</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="I36" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="B37" s="6" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D37" s="14" t="str">
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Camila</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G37" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>218</v>
+      </c>
       <c r="H37" s="12" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A13 B5:G5 I5 A14:G14 I14">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>$V4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A25">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$V15=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3">
-    <cfRule type="expression" dxfId="7" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$W3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:H4">
-    <cfRule type="expression" dxfId="6" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$V4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:H13">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>$V6=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:H25">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>$V15=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:G2">
-    <cfRule type="expression" dxfId="3" priority="21">
+    <cfRule type="expression" dxfId="14" priority="21">
       <formula>$W2=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="2" priority="16">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>$V5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I2">
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>$W2=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$V25=1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{C0737CE7-E542-4D1C-BA03-6991C3CF34C6}"/>
-    <hyperlink ref="I3" r:id="rId2" display="luis.gajardo@slepchiloe.gob.cl;" xr:uid="{8687092E-077F-44E0-8596-381E03D641E8}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{00B2325A-F588-41ED-AC5B-9DB5D89931CC}"/>
-    <hyperlink ref="H9" r:id="rId4" xr:uid="{13C55916-204E-4C3E-A397-C0E811E2FDC2}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{20C85ACE-7FF3-4FE2-BC88-162377C43342}"/>
-    <hyperlink ref="H12" r:id="rId6" xr:uid="{BB5038CA-BC9D-4D65-B196-5820788BA999}"/>
-    <hyperlink ref="I12" r:id="rId7" display="mailto:karla.sepulveda@sleppunillacordillera.cl" xr:uid="{FA9727FC-D1CA-4EF4-B723-4BF30F5C5E51}"/>
-    <hyperlink ref="H13" r:id="rId8" xr:uid="{0773547D-CCAE-4E00-A502-AB5D3C7A5D4F}"/>
-    <hyperlink ref="I14" r:id="rId9" xr:uid="{AC730A02-E5F5-4866-BC84-CA9DE3712292}"/>
-    <hyperlink ref="H14" r:id="rId10" xr:uid="{7231EF4D-AE48-4627-B0B7-6060424EA064}"/>
-    <hyperlink ref="H15" r:id="rId11" xr:uid="{CE4BA5E9-B40D-408E-A689-CDF23E66341C}"/>
-    <hyperlink ref="H16" r:id="rId12" xr:uid="{AEDEA0EB-604C-4C31-9304-42A01F8A5A3D}"/>
-    <hyperlink ref="H18" r:id="rId13" xr:uid="{F7398C85-77F6-4B2F-90F2-2305F57C2050}"/>
-    <hyperlink ref="H17" r:id="rId14" xr:uid="{5716803F-2B2A-4A17-BB69-8FDFE706A2AB}"/>
-    <hyperlink ref="H19" r:id="rId15" xr:uid="{E9048617-0AB9-404F-AD37-74E9A485BE30}"/>
-    <hyperlink ref="H20" r:id="rId16" xr:uid="{E454A7F1-60B0-46A2-BCAF-6EE451073594}"/>
-    <hyperlink ref="H21" r:id="rId17" xr:uid="{1127AC0B-364E-4EAD-9D99-A94EA5C42523}"/>
-    <hyperlink ref="H22" r:id="rId18" xr:uid="{898CFB37-C10F-4164-9DC8-B35726F71024}"/>
-    <hyperlink ref="H23" r:id="rId19" xr:uid="{9ECCB776-E8C3-4105-A6F7-2E6F2A184663}"/>
-    <hyperlink ref="H24" r:id="rId20" xr:uid="{4FC5ADBE-181E-43FF-9751-D6D427F0366F}"/>
-    <hyperlink ref="H25" r:id="rId21" xr:uid="{8A1E636A-763E-4FEA-AA46-C17108413427}"/>
-    <hyperlink ref="I25" r:id="rId22" xr:uid="{BC1D1921-7D71-457C-A023-855DF7FD4289}"/>
-    <hyperlink ref="H28" r:id="rId23" display="mailto:carolina.villagra@sleppetorca.gob.cl" xr:uid="{FA5AB3B0-F9E2-45ED-820A-9057AA7CB237}"/>
-    <hyperlink ref="H30" r:id="rId24" display="mailto:claudia.cubillos@slepaconcagua.gob.cl" xr:uid="{BF5D4A03-B565-4290-A323-81DEBCE5CFFB}"/>
-    <hyperlink ref="H31" r:id="rId25" display="mailto:javiera.rivas@sleppuelche.gob.cl" xr:uid="{0BE46A43-B5C0-4B49-A817-F11FCE265D50}"/>
-    <hyperlink ref="H32" r:id="rId26" display="mailto:claudio.wilson@sleplosalamos.gob.cl" xr:uid="{75417199-A8F7-4F2B-95A4-F7A17C2548B4}"/>
-    <hyperlink ref="H33" r:id="rId27" xr:uid="{54980B47-C332-416B-B63C-509B623066BB}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{EA77E657-6305-4130-AE9B-9278175D24E4}"/>
-    <hyperlink ref="H35" r:id="rId29" display="mailto:araceli.nunez@sleptamarugal.gob.cl" xr:uid="{A213DA54-6A21-4C6A-BAD1-5943AE13A95A}"/>
-    <hyperlink ref="I36" r:id="rId30" xr:uid="{A0920DFD-228F-41BB-9846-5BA8CD1645DD}"/>
-    <hyperlink ref="H37" r:id="rId31" xr:uid="{47683FAC-4633-465C-A962-957D7E10B3B6}"/>
-    <hyperlink ref="I37" r:id="rId32" xr:uid="{8A354AB1-E770-4F79-B1BA-93ADD65AA4C2}"/>
-    <hyperlink ref="I28" r:id="rId33" xr:uid="{874DA179-19F1-4B04-84DB-71FE5C56F6F3}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{00B2325A-F588-41ED-AC5B-9DB5D89931CC}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{13C55916-204E-4C3E-A397-C0E811E2FDC2}"/>
+    <hyperlink ref="H11" r:id="rId4" xr:uid="{20C85ACE-7FF3-4FE2-BC88-162377C43342}"/>
+    <hyperlink ref="H12" r:id="rId5" xr:uid="{BB5038CA-BC9D-4D65-B196-5820788BA999}"/>
+    <hyperlink ref="I12" r:id="rId6" display="mailto:karla.sepulveda@sleppunillacordillera.cl" xr:uid="{FA9727FC-D1CA-4EF4-B723-4BF30F5C5E51}"/>
+    <hyperlink ref="H13" r:id="rId7" xr:uid="{0773547D-CCAE-4E00-A502-AB5D3C7A5D4F}"/>
+    <hyperlink ref="I14" r:id="rId8" xr:uid="{AC730A02-E5F5-4866-BC84-CA9DE3712292}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{7231EF4D-AE48-4627-B0B7-6060424EA064}"/>
+    <hyperlink ref="H15" r:id="rId10" xr:uid="{CE4BA5E9-B40D-408E-A689-CDF23E66341C}"/>
+    <hyperlink ref="H16" r:id="rId11" xr:uid="{AEDEA0EB-604C-4C31-9304-42A01F8A5A3D}"/>
+    <hyperlink ref="H18" r:id="rId12" xr:uid="{F7398C85-77F6-4B2F-90F2-2305F57C2050}"/>
+    <hyperlink ref="H17" r:id="rId13" xr:uid="{5716803F-2B2A-4A17-BB69-8FDFE706A2AB}"/>
+    <hyperlink ref="H19" r:id="rId14" xr:uid="{E9048617-0AB9-404F-AD37-74E9A485BE30}"/>
+    <hyperlink ref="H20" r:id="rId15" xr:uid="{E454A7F1-60B0-46A2-BCAF-6EE451073594}"/>
+    <hyperlink ref="H21" r:id="rId16" xr:uid="{1127AC0B-364E-4EAD-9D99-A94EA5C42523}"/>
+    <hyperlink ref="H22" r:id="rId17" xr:uid="{898CFB37-C10F-4164-9DC8-B35726F71024}"/>
+    <hyperlink ref="H23" r:id="rId18" xr:uid="{9ECCB776-E8C3-4105-A6F7-2E6F2A184663}"/>
+    <hyperlink ref="H24" r:id="rId19" xr:uid="{4FC5ADBE-181E-43FF-9751-D6D427F0366F}"/>
+    <hyperlink ref="H25" r:id="rId20" xr:uid="{8A1E636A-763E-4FEA-AA46-C17108413427}"/>
+    <hyperlink ref="I25" r:id="rId21" xr:uid="{BC1D1921-7D71-457C-A023-855DF7FD4289}"/>
+    <hyperlink ref="H28" r:id="rId22" display="mailto:carolina.villagra@sleppetorca.gob.cl" xr:uid="{FA5AB3B0-F9E2-45ED-820A-9057AA7CB237}"/>
+    <hyperlink ref="H30" r:id="rId23" display="mailto:claudia.cubillos@slepaconcagua.gob.cl" xr:uid="{BF5D4A03-B565-4290-A323-81DEBCE5CFFB}"/>
+    <hyperlink ref="H32" r:id="rId24" display="mailto:claudio.wilson@sleplosalamos.gob.cl" xr:uid="{75417199-A8F7-4F2B-95A4-F7A17C2548B4}"/>
+    <hyperlink ref="H33" r:id="rId25" xr:uid="{54980B47-C332-416B-B63C-509B623066BB}"/>
+    <hyperlink ref="H34" r:id="rId26" xr:uid="{EA77E657-6305-4130-AE9B-9278175D24E4}"/>
+    <hyperlink ref="H35" r:id="rId27" display="mailto:araceli.nunez@sleptamarugal.gob.cl" xr:uid="{A213DA54-6A21-4C6A-BAD1-5943AE13A95A}"/>
+    <hyperlink ref="I36" r:id="rId28" xr:uid="{A0920DFD-228F-41BB-9846-5BA8CD1645DD}"/>
+    <hyperlink ref="H37" r:id="rId29" xr:uid="{47683FAC-4633-465C-A962-957D7E10B3B6}"/>
+    <hyperlink ref="I37" r:id="rId30" xr:uid="{8A354AB1-E770-4F79-B1BA-93ADD65AA4C2}"/>
+    <hyperlink ref="I28" r:id="rId31" xr:uid="{874DA179-19F1-4B04-84DB-71FE5C56F6F3}"/>
+    <hyperlink ref="I31" r:id="rId32" xr:uid="{23A89A35-5FE5-4753-8C1C-C063A7CCAF17}"/>
+    <hyperlink ref="H31" r:id="rId33" xr:uid="{8CE3801F-2D31-452D-923C-A8593A3AA3A3}"/>
+    <hyperlink ref="H36" r:id="rId34" xr:uid="{5E6E2E2A-9007-46B7-9964-2E09249D8F3A}"/>
+    <hyperlink ref="I34" r:id="rId35" xr:uid="{0011810F-DE97-45D0-9471-2DE01C3A5189}"/>
+    <hyperlink ref="I30" r:id="rId36" xr:uid="{A7A1E120-0ED5-475C-A8BB-BE81B51B7066}"/>
+    <hyperlink ref="I32" r:id="rId37" xr:uid="{301B3643-4756-45C1-BC55-FF9FD4821B41}"/>
+    <hyperlink ref="I29" r:id="rId38" xr:uid="{129AB270-59C0-4501-B6EC-9626D7FC587B}"/>
+    <hyperlink ref="I33" r:id="rId39" xr:uid="{9621396B-EE77-4EC0-85EA-D9CF2492F76D}"/>
+    <hyperlink ref="I35" r:id="rId40" xr:uid="{7B46DDAA-2840-4B7C-806A-9D8C13D76907}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId34"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId41"/>
   <tableParts count="1">
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId42"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2645,136 +2782,136 @@
       <selection sqref="A1:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2786,9 +2923,5 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD8AD7E-D7E2-48EE-A5BD-CE862A98C9B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD8AD7E-D7E2-48EE-A5BD-CE862A98C9B8}"/>
 </file>
</xml_diff>